<commit_message>
Updated exception for excel sheet opening errors.
</commit_message>
<xml_diff>
--- a/StudentDetails.xlsx
+++ b/StudentDetails.xlsx
@@ -411,7 +411,7 @@
       <selection activeCell="A1" sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
@@ -539,13 +539,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
@@ -636,7 +636,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>11-1-1997</t>
+          <t>11-01-1997</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -654,8 +654,10 @@
           <t>31</t>
         </is>
       </c>
-      <c r="G2" t="n">
-        <v>43</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -672,10 +674,8 @@
           <t>100</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
+      <c r="K2" t="n">
+        <v>324</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -696,7 +696,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>11-1-1998</t>
+          <t>11-01-1998</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -734,14 +734,72 @@
           <t>45</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>373</t>
-        </is>
+      <c r="K3" t="n">
+        <v>373</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Stephan</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>08-09-1996</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>275</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>F</t>
         </is>
       </c>
     </row>
@@ -762,7 +820,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
@@ -942,7 +1000,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
@@ -1217,20 +1275,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="11.42578125" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
     <col width="30" customWidth="1" min="5" max="5"/>
     <col width="20" customWidth="1" min="6" max="12"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1308,7 +1372,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1991-07-11</t>
+          <t>10-09-1991</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1323,14 +1387,14 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>31</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>31</t>
-        </is>
-      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>100</t>
@@ -1347,11 +1411,11 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>312</v>
+        <v>381</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -1368,7 +1432,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1991-07-12</t>
+          <t>10-05-1994</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1412,6 +1476,66 @@
       <c r="L3" t="inlineStr">
         <is>
           <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Jofin</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>10-09-2022</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Pulickal</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>68</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>412</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -1426,19 +1550,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="3"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="5"/>
-    <col width="40" customWidth="1" min="6" max="6"/>
-    <col width="50" customWidth="1" min="7" max="7"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1516,7 +1647,8 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1991-07-11</t>
+          <t xml:space="preserve">02-04-1990
+</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1554,10 +1686,8 @@
           <t>100</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
+      <c r="K2" t="n">
+        <v>312</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -1578,7 +1708,8 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1991-07-12</t>
+          <t xml:space="preserve">22-08-1999
+</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1616,14 +1747,72 @@
           <t>10</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
+      <c r="K3" t="n">
+        <v>103</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Joseph</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12-08-1994</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Munich</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>76</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>66</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>428</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>B</t>
         </is>
       </c>
     </row>
@@ -1644,7 +1833,7 @@
       <selection activeCell="A1" sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
@@ -1779,7 +1968,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="3"/>
@@ -1913,7 +2102,7 @@
       <selection activeCell="A1" sqref="A1:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
@@ -2093,7 +2282,7 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="30" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="3"/>

</xml_diff>

<commit_message>
added comments and formatted Code.
</commit_message>
<xml_diff>
--- a/StudentDetails.xlsx
+++ b/StudentDetails.xlsx
@@ -994,7 +994,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -1261,6 +1261,66 @@
       <c r="L4" t="inlineStr">
         <is>
           <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Luke</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>12-01-2000</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>USA</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>77</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>408</v>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>B</t>
         </is>
       </c>
     </row>

</xml_diff>